<commit_message>
calorimetry : scripts : data load
</commit_message>
<xml_diff>
--- a/input/calorimetry/ds.1.dsc/test_1.xlsx
+++ b/input/calorimetry/ds.1.dsc/test_1.xlsx
@@ -5,16 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="input_stoich_coefficients" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="input_k_constants_log10" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="input_concentrations" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="component_name" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="heats" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="targets" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="enthalpies" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="heats" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="targets" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="enthalpies" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t xml:space="preserve">PLP</t>
   </si>
@@ -463,20 +462,267 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="2" style="0" width="26.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="17" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="C1" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="N1" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="O1" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="P1" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>15.024997</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>15.049994</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>15.074991</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>15.099988</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>15.124985</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <v>15.149982</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>15.174979</v>
+      </c>
+      <c r="I2" s="3" t="n">
+        <v>15.199976</v>
+      </c>
+      <c r="J2" s="3" t="n">
+        <v>15.224973</v>
+      </c>
+      <c r="K2" s="3" t="n">
+        <v>15.24997</v>
+      </c>
+      <c r="L2" s="3" t="n">
+        <v>15.274967</v>
+      </c>
+      <c r="M2" s="3" t="n">
+        <v>15.299964</v>
+      </c>
+      <c r="N2" s="3" t="n">
+        <v>15.324961</v>
+      </c>
+      <c r="O2" s="3" t="n">
+        <v>15.349958</v>
+      </c>
+      <c r="P2" s="3" t="n">
+        <v>15.374955</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>0.069951</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>0.069513</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>0.069854</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>0.071474</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>0.067108</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>0.066289</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>0.056026</v>
+      </c>
+      <c r="I3" s="3" t="n">
+        <v>0.044493</v>
+      </c>
+      <c r="J3" s="3" t="n">
+        <v>0.027882</v>
+      </c>
+      <c r="K3" s="3" t="n">
+        <v>0.009239</v>
+      </c>
+      <c r="L3" s="3" t="n">
+        <v>0.003057</v>
+      </c>
+      <c r="M3" s="3" t="n">
+        <v>0.002486</v>
+      </c>
+      <c r="N3" s="3" t="n">
+        <v>0.000906</v>
+      </c>
+      <c r="O3" s="3" t="n">
+        <v>4E-005</v>
+      </c>
+      <c r="P3" s="3" t="n">
+        <v>-0.001894</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>-0.001953538</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>0.002471029</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>-0.00017689</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>0.000556654</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>0.00070773</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>0.001854236</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <v>0.001081072</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <v>0.000473122</v>
+      </c>
+      <c r="J4" s="3" t="n">
+        <v>0.00106313</v>
+      </c>
+      <c r="K4" s="3" t="n">
+        <v>0.000271799</v>
+      </c>
+      <c r="L4" s="3" t="n">
+        <v>0.001168423</v>
+      </c>
+      <c r="M4" s="3" t="n">
+        <v>0.000232129</v>
+      </c>
+      <c r="N4" s="3" t="n">
+        <v>0.000917353</v>
+      </c>
+      <c r="O4" s="3" t="n">
+        <v>0.001269958</v>
+      </c>
+      <c r="P4" s="3" t="n">
+        <v>-0.000397241</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="I5" s="3" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="J5" s="3" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="K5" s="3" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="L5" s="3" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="M5" s="3" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="N5" s="3" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="O5" s="3" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="P5" s="3" t="n">
+        <v>1E-006</v>
       </c>
     </row>
   </sheetData>
@@ -495,267 +741,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="2" style="0" width="26.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="17" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F1" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="G1" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="H1" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="I1" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="J1" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="K1" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="L1" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="M1" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="N1" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="O1" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="P1" s="0" t="n">
-        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="3" t="n">
-        <v>15.024997</v>
-      </c>
-      <c r="C2" s="3" t="n">
-        <v>15.049994</v>
-      </c>
-      <c r="D2" s="3" t="n">
-        <v>15.074991</v>
-      </c>
-      <c r="E2" s="3" t="n">
-        <v>15.099988</v>
-      </c>
-      <c r="F2" s="3" t="n">
-        <v>15.124985</v>
-      </c>
-      <c r="G2" s="3" t="n">
-        <v>15.149982</v>
-      </c>
-      <c r="H2" s="3" t="n">
-        <v>15.174979</v>
-      </c>
-      <c r="I2" s="3" t="n">
-        <v>15.199976</v>
-      </c>
-      <c r="J2" s="3" t="n">
-        <v>15.224973</v>
-      </c>
-      <c r="K2" s="3" t="n">
-        <v>15.24997</v>
-      </c>
-      <c r="L2" s="3" t="n">
-        <v>15.274967</v>
-      </c>
-      <c r="M2" s="3" t="n">
-        <v>15.299964</v>
-      </c>
-      <c r="N2" s="3" t="n">
-        <v>15.324961</v>
-      </c>
-      <c r="O2" s="3" t="n">
-        <v>15.349958</v>
-      </c>
-      <c r="P2" s="3" t="n">
-        <v>15.374955</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3" t="n">
-        <v>0.069951</v>
-      </c>
-      <c r="C3" s="3" t="n">
-        <v>0.069513</v>
-      </c>
-      <c r="D3" s="3" t="n">
-        <v>0.069854</v>
-      </c>
-      <c r="E3" s="3" t="n">
-        <v>0.071474</v>
-      </c>
-      <c r="F3" s="3" t="n">
-        <v>0.067108</v>
-      </c>
-      <c r="G3" s="3" t="n">
-        <v>0.066289</v>
-      </c>
-      <c r="H3" s="3" t="n">
-        <v>0.056026</v>
-      </c>
-      <c r="I3" s="3" t="n">
-        <v>0.044493</v>
-      </c>
-      <c r="J3" s="3" t="n">
-        <v>0.027882</v>
-      </c>
-      <c r="K3" s="3" t="n">
-        <v>0.009239</v>
-      </c>
-      <c r="L3" s="3" t="n">
-        <v>0.003057</v>
-      </c>
-      <c r="M3" s="3" t="n">
-        <v>0.002486</v>
-      </c>
-      <c r="N3" s="3" t="n">
-        <v>0.000906</v>
-      </c>
-      <c r="O3" s="3" t="n">
-        <v>4E-005</v>
-      </c>
-      <c r="P3" s="3" t="n">
-        <v>-0.001894</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="3" t="n">
-        <v>-0.001953538</v>
-      </c>
-      <c r="C4" s="3" t="n">
-        <v>0.002471029</v>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>-0.00017689</v>
-      </c>
-      <c r="E4" s="3" t="n">
-        <v>0.000556654</v>
-      </c>
-      <c r="F4" s="3" t="n">
-        <v>0.00070773</v>
-      </c>
-      <c r="G4" s="3" t="n">
-        <v>0.001854236</v>
-      </c>
-      <c r="H4" s="3" t="n">
-        <v>0.001081072</v>
-      </c>
-      <c r="I4" s="3" t="n">
-        <v>0.000473122</v>
-      </c>
-      <c r="J4" s="3" t="n">
-        <v>0.00106313</v>
-      </c>
-      <c r="K4" s="3" t="n">
-        <v>0.000271799</v>
-      </c>
-      <c r="L4" s="3" t="n">
-        <v>0.001168423</v>
-      </c>
-      <c r="M4" s="3" t="n">
-        <v>0.000232129</v>
-      </c>
-      <c r="N4" s="3" t="n">
-        <v>0.000917353</v>
-      </c>
-      <c r="O4" s="3" t="n">
-        <v>0.001269958</v>
-      </c>
-      <c r="P4" s="3" t="n">
-        <v>-0.000397241</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="3" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="C5" s="3" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="D5" s="3" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="E5" s="3" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="F5" s="3" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="G5" s="3" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="H5" s="3" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="I5" s="3" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="J5" s="3" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="K5" s="3" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="L5" s="3" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="M5" s="3" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="N5" s="3" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="O5" s="3" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="P5" s="3" t="n">
-        <v>1E-006</v>
+        <v>12</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -770,49 +780,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>

</xml_diff>

<commit_message>
calorimetry : scripts : data load : all setup info accumulated into setup file/sheet
</commit_message>
<xml_diff>
--- a/input/calorimetry/ds.1.dsc/test_1.xlsx
+++ b/input/calorimetry/ds.1.dsc/test_1.xlsx
@@ -12,9 +12,8 @@
     <sheet name="input_k_constants_log10" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="input_concentrations" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="heats" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="targets" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="enthalpies" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="setup" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="enthalpies" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="setup" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -61,25 +60,25 @@
     <t xml:space="preserve">deviation</t>
   </si>
   <si>
+    <t xml:space="preserve">Reaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calorimeter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DSC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">component</t>
+  </si>
+  <si>
     <t xml:space="preserve">constants </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reaction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calorimeter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DSC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Initial volume</t>
-  </si>
-  <si>
-    <t xml:space="preserve">component</t>
   </si>
 </sst>
 </file>
@@ -747,7 +746,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -760,7 +759,7 @@
         <v>11</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -779,42 +778,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
@@ -827,15 +791,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>15</v>
@@ -843,10 +807,18 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>